<commit_message>
updated excel spreadsheet for serial events and commands
</commit_message>
<xml_diff>
--- a/docs/serial_interface.xlsx
+++ b/docs/serial_interface.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
   <si>
     <t>Commands</t>
   </si>
@@ -226,6 +226,36 @@
   </si>
   <si>
     <t>From nRF51 to host</t>
+  </si>
+  <si>
+    <t>radio reset</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>Immediately resets device, which then generates a DEVICE_STARTED event</t>
+  </si>
+  <si>
+    <t>DEVICE_STARTED</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>0x81</t>
+  </si>
+  <si>
+    <t>M: Operating mode, E: HW error, D: Data credit available</t>
   </si>
 </sst>
 </file>
@@ -390,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -468,6 +498,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,24 +531,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -797,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AQ29"/>
+  <dimension ref="A2:AQ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,6 +1000,9 @@
       <c r="AN3" s="9"/>
       <c r="AO3" s="9"/>
       <c r="AP3" s="9"/>
+      <c r="AQ3" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -971,37 +1017,37 @@
       <c r="E4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
-      <c r="AG4" s="36"/>
-      <c r="AH4" s="37"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="32"/>
+      <c r="AB4" s="32"/>
+      <c r="AC4" s="32"/>
+      <c r="AD4" s="32"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
+      <c r="AG4" s="32"/>
+      <c r="AH4" s="33"/>
       <c r="AI4" s="26"/>
       <c r="AJ4" s="27"/>
       <c r="AK4" s="27"/>
@@ -1010,119 +1056,150 @@
       <c r="AN4" s="27"/>
       <c r="AO4" s="27"/>
       <c r="AP4" s="27"/>
-      <c r="AQ4" s="1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="5" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="41">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="12">
-        <v>11</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="34"/>
-      <c r="AI5" s="9"/>
-      <c r="AQ5" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="27"/>
+      <c r="AF5" s="27"/>
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="27"/>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="27"/>
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="27"/>
+      <c r="AO5" s="27"/>
+      <c r="AP5" s="27"/>
+      <c r="AQ5" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>58</v>
+      <c r="D6" s="12">
+        <v>11</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="30"/>
-      <c r="AB6" s="30"/>
-      <c r="AC6" s="30"/>
-      <c r="AD6" s="30"/>
-      <c r="AE6" s="30"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
-      <c r="AH6" s="31"/>
+        <v>26</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="36"/>
+      <c r="AI6" s="9"/>
       <c r="AQ6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="12">
-        <v>2</v>
+      <c r="D7" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="38"/>
+      <c r="AB7" s="38"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="38"/>
+      <c r="AE7" s="38"/>
+      <c r="AF7" s="38"/>
+      <c r="AG7" s="38"/>
+      <c r="AH7" s="39"/>
       <c r="AQ7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -1131,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>12</v>
@@ -1141,133 +1218,107 @@
       </c>
     </row>
     <row r="9" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="D9" s="25"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="10"/>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="12">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="13">
-        <v>2</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="9"/>
-      <c r="AG10" s="9"/>
-      <c r="AH10" s="9"/>
-      <c r="AQ10" t="s">
-        <v>62</v>
-      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="12">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="D11" s="13">
+        <v>2</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>39</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
       <c r="AQ11" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
+        <v>39</v>
+      </c>
       <c r="AQ12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="12">
         <v>1</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -1299,21 +1350,21 @@
       <c r="AG13" s="9"/>
       <c r="AH13" s="9"/>
       <c r="AQ13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D14" s="12">
         <v>1</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -1350,16 +1401,16 @@
     </row>
     <row r="15" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="12">
         <v>1</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -1391,12 +1442,22 @@
       <c r="AG15" s="9"/>
       <c r="AH15" s="9"/>
       <c r="AQ15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="D16" s="23"/>
-      <c r="E16" s="20"/>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -1426,6 +1487,9 @@
       <c r="AF16" s="9"/>
       <c r="AG16" s="9"/>
       <c r="AH16" s="9"/>
+      <c r="AQ16" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D17" s="23"/>
@@ -1593,254 +1657,204 @@
       <c r="AH21" s="9"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="D22" s="23"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="19"/>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1"/>
       <c r="D23" s="19"/>
-      <c r="AI23" s="9"/>
-      <c r="AJ23" s="9"/>
-      <c r="AK23" s="9"/>
-      <c r="AL23" s="9"/>
-      <c r="AM23" s="9"/>
-      <c r="AN23" s="9"/>
-      <c r="AO23" s="9"/>
-      <c r="AP23" s="9"/>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="19"/>
+      <c r="AI24" s="9"/>
+      <c r="AJ24" s="9"/>
+      <c r="AK24" s="9"/>
+      <c r="AL24" s="9"/>
+      <c r="AM24" s="9"/>
+      <c r="AN24" s="9"/>
+      <c r="AO24" s="9"/>
+      <c r="AP24" s="9"/>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="42">
+        <v>4</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI25" s="29"/>
+      <c r="AJ25" s="29"/>
+      <c r="AK25" s="29"/>
+      <c r="AL25" s="29"/>
+      <c r="AM25" s="29"/>
+      <c r="AN25" s="29"/>
+      <c r="AO25" s="29"/>
+      <c r="AP25" s="29"/>
+      <c r="AQ25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="17" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F26" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="36"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="36"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
-      <c r="AA24" s="36"/>
-      <c r="AB24" s="36"/>
-      <c r="AC24" s="36"/>
-      <c r="AD24" s="36"/>
-      <c r="AE24" s="36"/>
-      <c r="AF24" s="36"/>
-      <c r="AG24" s="36"/>
-      <c r="AH24" s="36"/>
-      <c r="AI24" s="26"/>
-      <c r="AJ24" s="27"/>
-      <c r="AK24" s="27"/>
-      <c r="AL24" s="27"/>
-      <c r="AM24" s="27"/>
-      <c r="AN24" s="27"/>
-      <c r="AO24" s="27"/>
-      <c r="AP24" s="27"/>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="30"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="30"/>
-      <c r="AB25" s="30"/>
-      <c r="AC25" s="30"/>
-      <c r="AD25" s="30"/>
-      <c r="AE25" s="30"/>
-      <c r="AF25" s="30"/>
-      <c r="AG25" s="30"/>
-      <c r="AH25" s="30"/>
-      <c r="AI25" s="8"/>
-      <c r="AQ25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H26" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30"/>
-      <c r="AA26" s="30"/>
-      <c r="AB26" s="30"/>
-      <c r="AC26" s="30"/>
-      <c r="AD26" s="30"/>
-      <c r="AE26" s="30"/>
-      <c r="AF26" s="30"/>
-      <c r="AG26" s="30"/>
-      <c r="AH26" s="30"/>
-      <c r="AI26" s="30"/>
-      <c r="AJ26" s="30"/>
-      <c r="AK26" s="30"/>
-      <c r="AL26" s="30"/>
-      <c r="AM26" s="30"/>
-      <c r="AN26" s="30"/>
-      <c r="AO26" s="31"/>
-      <c r="AQ26" t="s">
-        <v>60</v>
-      </c>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="32"/>
+      <c r="V26" s="32"/>
+      <c r="W26" s="32"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="32"/>
+      <c r="Z26" s="32"/>
+      <c r="AA26" s="32"/>
+      <c r="AB26" s="32"/>
+      <c r="AC26" s="32"/>
+      <c r="AD26" s="32"/>
+      <c r="AE26" s="32"/>
+      <c r="AF26" s="32"/>
+      <c r="AG26" s="32"/>
+      <c r="AH26" s="32"/>
+      <c r="AI26" s="26"/>
+      <c r="AJ26" s="27"/>
+      <c r="AK26" s="27"/>
+      <c r="AL26" s="27"/>
+      <c r="AM26" s="27"/>
+      <c r="AN26" s="27"/>
+      <c r="AO26" s="27"/>
+      <c r="AP26" s="27"/>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H27" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="30"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="30"/>
-      <c r="AA27" s="30"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="30"/>
-      <c r="AE27" s="30"/>
-      <c r="AF27" s="30"/>
-      <c r="AG27" s="30"/>
-      <c r="AH27" s="30"/>
-      <c r="AI27" s="30"/>
-      <c r="AJ27" s="30"/>
-      <c r="AK27" s="30"/>
-      <c r="AL27" s="30"/>
-      <c r="AM27" s="30"/>
-      <c r="AN27" s="30"/>
-      <c r="AO27" s="31"/>
+        <v>19</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="38"/>
+      <c r="V27" s="38"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="38"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="38"/>
+      <c r="AB27" s="38"/>
+      <c r="AC27" s="38"/>
+      <c r="AD27" s="38"/>
+      <c r="AE27" s="38"/>
+      <c r="AF27" s="38"/>
+      <c r="AG27" s="38"/>
+      <c r="AH27" s="38"/>
+      <c r="AI27" s="8"/>
       <c r="AQ27" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>64</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>12</v>
@@ -1848,71 +1862,187 @@
       <c r="G28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H28" s="29" t="s">
+      <c r="H28" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="29" t="s">
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="30"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="30"/>
-      <c r="Z28" s="30"/>
-      <c r="AA28" s="30"/>
-      <c r="AB28" s="30"/>
-      <c r="AC28" s="30"/>
-      <c r="AD28" s="30"/>
-      <c r="AE28" s="30"/>
-      <c r="AF28" s="30"/>
-      <c r="AG28" s="30"/>
-      <c r="AH28" s="30"/>
-      <c r="AI28" s="30"/>
-      <c r="AJ28" s="30"/>
-      <c r="AK28" s="30"/>
-      <c r="AL28" s="30"/>
-      <c r="AM28" s="30"/>
-      <c r="AN28" s="30"/>
-      <c r="AO28" s="31"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="38"/>
+      <c r="T28" s="38"/>
+      <c r="U28" s="38"/>
+      <c r="V28" s="38"/>
+      <c r="W28" s="38"/>
+      <c r="X28" s="38"/>
+      <c r="Y28" s="38"/>
+      <c r="Z28" s="38"/>
+      <c r="AA28" s="38"/>
+      <c r="AB28" s="38"/>
+      <c r="AC28" s="38"/>
+      <c r="AD28" s="38"/>
+      <c r="AE28" s="38"/>
+      <c r="AF28" s="38"/>
+      <c r="AG28" s="38"/>
+      <c r="AH28" s="38"/>
+      <c r="AI28" s="38"/>
+      <c r="AJ28" s="38"/>
+      <c r="AK28" s="38"/>
+      <c r="AL28" s="38"/>
+      <c r="AM28" s="38"/>
+      <c r="AN28" s="38"/>
+      <c r="AO28" s="39"/>
       <c r="AQ28" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D29" s="21"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="38"/>
+      <c r="U29" s="38"/>
+      <c r="V29" s="38"/>
+      <c r="W29" s="38"/>
+      <c r="X29" s="38"/>
+      <c r="Y29" s="38"/>
+      <c r="Z29" s="38"/>
+      <c r="AA29" s="38"/>
+      <c r="AB29" s="38"/>
+      <c r="AC29" s="38"/>
+      <c r="AD29" s="38"/>
+      <c r="AE29" s="38"/>
+      <c r="AF29" s="38"/>
+      <c r="AG29" s="38"/>
+      <c r="AH29" s="38"/>
+      <c r="AI29" s="38"/>
+      <c r="AJ29" s="38"/>
+      <c r="AK29" s="38"/>
+      <c r="AL29" s="38"/>
+      <c r="AM29" s="38"/>
+      <c r="AN29" s="38"/>
+      <c r="AO29" s="39"/>
+      <c r="AQ29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H30" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="38"/>
+      <c r="U30" s="38"/>
+      <c r="V30" s="38"/>
+      <c r="W30" s="38"/>
+      <c r="X30" s="38"/>
+      <c r="Y30" s="38"/>
+      <c r="Z30" s="38"/>
+      <c r="AA30" s="38"/>
+      <c r="AB30" s="38"/>
+      <c r="AC30" s="38"/>
+      <c r="AD30" s="38"/>
+      <c r="AE30" s="38"/>
+      <c r="AF30" s="38"/>
+      <c r="AG30" s="38"/>
+      <c r="AH30" s="38"/>
+      <c r="AI30" s="38"/>
+      <c r="AJ30" s="38"/>
+      <c r="AK30" s="38"/>
+      <c r="AL30" s="38"/>
+      <c r="AM30" s="38"/>
+      <c r="AN30" s="38"/>
+      <c r="AO30" s="39"/>
+      <c r="AQ30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="D31" s="21"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="N29:AO29"/>
+    <mergeCell ref="N30:AO30"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="N28:AO28"/>
     <mergeCell ref="F4:AH4"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="G6:AH6"/>
-    <mergeCell ref="H25:AH25"/>
-    <mergeCell ref="F24:AH24"/>
-    <mergeCell ref="N27:AO27"/>
-    <mergeCell ref="N28:AO28"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="N26:AO26"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="G7:AH7"/>
+    <mergeCell ref="H27:AH27"/>
+    <mergeCell ref="F26:AH26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added start/stop commands to serial interface command overview
</commit_message>
<xml_diff>
--- a/docs/serial_interface.xlsx
+++ b/docs/serial_interface.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="84">
   <si>
     <t>Commands</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>M: Operating mode, E: HW error, D: Data credit available</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>0x74</t>
+  </si>
+  <si>
+    <t>0x75</t>
   </si>
 </sst>
 </file>
@@ -297,7 +309,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -415,12 +427,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -507,37 +530,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -840,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AQ31"/>
+  <dimension ref="A2:AQ33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,37 +1049,37 @@
       <c r="E4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="32"/>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="32"/>
-      <c r="AF4" s="32"/>
-      <c r="AG4" s="32"/>
-      <c r="AH4" s="33"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="39"/>
       <c r="AI4" s="26"/>
       <c r="AJ4" s="27"/>
       <c r="AK4" s="27"/>
@@ -1064,7 +1096,7 @@
       <c r="C5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="33">
         <v>1</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -1124,24 +1156,24 @@
       <c r="E6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="36"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="42"/>
       <c r="AI6" s="9"/>
       <c r="AQ6" t="s">
         <v>61</v>
@@ -1163,36 +1195,36 @@
       <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="38"/>
-      <c r="AC7" s="38"/>
-      <c r="AD7" s="38"/>
-      <c r="AE7" s="38"/>
-      <c r="AF7" s="38"/>
-      <c r="AG7" s="38"/>
-      <c r="AH7" s="39"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="36"/>
+      <c r="X7" s="36"/>
+      <c r="Y7" s="36"/>
+      <c r="Z7" s="36"/>
+      <c r="AA7" s="36"/>
+      <c r="AB7" s="36"/>
+      <c r="AC7" s="36"/>
+      <c r="AD7" s="36"/>
+      <c r="AE7" s="36"/>
+      <c r="AF7" s="36"/>
+      <c r="AG7" s="36"/>
+      <c r="AH7" s="37"/>
       <c r="AQ7" t="s">
         <v>66</v>
       </c>
@@ -1238,89 +1270,56 @@
       </c>
     </row>
     <row r="10" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="D10" s="25"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="10"/>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="44"/>
     </row>
     <row r="11" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="13">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="9"/>
-      <c r="AH11" s="9"/>
-      <c r="AQ11" t="s">
-        <v>62</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="F11" s="45"/>
     </row>
     <row r="12" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ12" t="s">
-        <v>53</v>
-      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="12">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="D13" s="13">
+        <v>2</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1350,67 +1349,38 @@
       <c r="AG13" s="9"/>
       <c r="AH13" s="9"/>
       <c r="AQ13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="12">
         <v>1</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
+        <v>39</v>
+      </c>
       <c r="AQ14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D15" s="12">
         <v>1</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -1442,21 +1412,21 @@
       <c r="AG15" s="9"/>
       <c r="AH15" s="9"/>
       <c r="AQ15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D16" s="12">
         <v>1</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -1488,12 +1458,22 @@
       <c r="AG16" s="9"/>
       <c r="AH16" s="9"/>
       <c r="AQ16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D17" s="23"/>
-      <c r="E17" s="20"/>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="12">
+        <v>1</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -1523,10 +1503,23 @@
       <c r="AF17" s="9"/>
       <c r="AG17" s="9"/>
       <c r="AH17" s="9"/>
+      <c r="AQ17" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D18" s="23"/>
-      <c r="E18" s="20"/>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -1556,6 +1549,9 @@
       <c r="AF18" s="9"/>
       <c r="AG18" s="9"/>
       <c r="AH18" s="9"/>
+      <c r="AQ18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D19" s="23"/>
@@ -1690,189 +1686,149 @@
       <c r="AH22" s="9"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="D23" s="23"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="9"/>
+      <c r="AC23" s="9"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="19"/>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="19"/>
-      <c r="AI24" s="9"/>
-      <c r="AJ24" s="9"/>
-      <c r="AK24" s="9"/>
-      <c r="AL24" s="9"/>
-      <c r="AM24" s="9"/>
-      <c r="AN24" s="9"/>
-      <c r="AO24" s="9"/>
-      <c r="AP24" s="9"/>
-    </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="42">
-        <v>4</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI25" s="29"/>
-      <c r="AJ25" s="29"/>
-      <c r="AK25" s="29"/>
-      <c r="AL25" s="29"/>
-      <c r="AM25" s="29"/>
-      <c r="AN25" s="29"/>
-      <c r="AO25" s="29"/>
-      <c r="AP25" s="29"/>
-      <c r="AQ25" t="s">
-        <v>79</v>
-      </c>
+      <c r="D25" s="19"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="19"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="9"/>
+      <c r="AK26" s="9"/>
+      <c r="AL26" s="9"/>
+      <c r="AM26" s="9"/>
+      <c r="AN26" s="9"/>
+      <c r="AO26" s="9"/>
+      <c r="AP26" s="9"/>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="34">
+        <v>4</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="29"/>
+      <c r="AN27" s="29"/>
+      <c r="AO27" s="29"/>
+      <c r="AP27" s="29"/>
+      <c r="AQ27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="17" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F28" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="32"/>
-      <c r="S26" s="32"/>
-      <c r="T26" s="32"/>
-      <c r="U26" s="32"/>
-      <c r="V26" s="32"/>
-      <c r="W26" s="32"/>
-      <c r="X26" s="32"/>
-      <c r="Y26" s="32"/>
-      <c r="Z26" s="32"/>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="32"/>
-      <c r="AC26" s="32"/>
-      <c r="AD26" s="32"/>
-      <c r="AE26" s="32"/>
-      <c r="AF26" s="32"/>
-      <c r="AG26" s="32"/>
-      <c r="AH26" s="32"/>
-      <c r="AI26" s="26"/>
-      <c r="AJ26" s="27"/>
-      <c r="AK26" s="27"/>
-      <c r="AL26" s="27"/>
-      <c r="AM26" s="27"/>
-      <c r="AN26" s="27"/>
-      <c r="AO26" s="27"/>
-      <c r="AP26" s="27"/>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="38"/>
-      <c r="V27" s="38"/>
-      <c r="W27" s="38"/>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38"/>
-      <c r="Z27" s="38"/>
-      <c r="AA27" s="38"/>
-      <c r="AB27" s="38"/>
-      <c r="AC27" s="38"/>
-      <c r="AD27" s="38"/>
-      <c r="AE27" s="38"/>
-      <c r="AF27" s="38"/>
-      <c r="AG27" s="38"/>
-      <c r="AH27" s="38"/>
-      <c r="AI27" s="8"/>
-      <c r="AQ27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H28" s="37" t="s">
-        <v>20</v>
-      </c>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
       <c r="I28" s="38"/>
       <c r="J28" s="38"/>
       <c r="K28" s="38"/>
       <c r="L28" s="38"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="37" t="s">
-        <v>13</v>
-      </c>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
       <c r="O28" s="38"/>
       <c r="P28" s="38"/>
       <c r="Q28" s="38"/>
@@ -1893,84 +1849,74 @@
       <c r="AF28" s="38"/>
       <c r="AG28" s="38"/>
       <c r="AH28" s="38"/>
-      <c r="AI28" s="38"/>
-      <c r="AJ28" s="38"/>
-      <c r="AK28" s="38"/>
-      <c r="AL28" s="38"/>
-      <c r="AM28" s="38"/>
-      <c r="AN28" s="38"/>
-      <c r="AO28" s="39"/>
-      <c r="AQ28" t="s">
-        <v>60</v>
-      </c>
+      <c r="AI28" s="26"/>
+      <c r="AJ28" s="27"/>
+      <c r="AK28" s="27"/>
+      <c r="AL28" s="27"/>
+      <c r="AM28" s="27"/>
+      <c r="AN28" s="27"/>
+      <c r="AO28" s="27"/>
+      <c r="AP28" s="27"/>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H29" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="O29" s="38"/>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="38"/>
-      <c r="R29" s="38"/>
-      <c r="S29" s="38"/>
-      <c r="T29" s="38"/>
-      <c r="U29" s="38"/>
-      <c r="V29" s="38"/>
-      <c r="W29" s="38"/>
-      <c r="X29" s="38"/>
-      <c r="Y29" s="38"/>
-      <c r="Z29" s="38"/>
-      <c r="AA29" s="38"/>
-      <c r="AB29" s="38"/>
-      <c r="AC29" s="38"/>
-      <c r="AD29" s="38"/>
-      <c r="AE29" s="38"/>
-      <c r="AF29" s="38"/>
-      <c r="AG29" s="38"/>
-      <c r="AH29" s="38"/>
-      <c r="AI29" s="38"/>
-      <c r="AJ29" s="38"/>
-      <c r="AK29" s="38"/>
-      <c r="AL29" s="38"/>
-      <c r="AM29" s="38"/>
-      <c r="AN29" s="38"/>
-      <c r="AO29" s="39"/>
+        <v>19</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="36"/>
+      <c r="U29" s="36"/>
+      <c r="V29" s="36"/>
+      <c r="W29" s="36"/>
+      <c r="X29" s="36"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36"/>
+      <c r="AA29" s="36"/>
+      <c r="AB29" s="36"/>
+      <c r="AC29" s="36"/>
+      <c r="AD29" s="36"/>
+      <c r="AE29" s="36"/>
+      <c r="AF29" s="36"/>
+      <c r="AG29" s="36"/>
+      <c r="AH29" s="36"/>
+      <c r="AI29" s="8"/>
       <c r="AQ29" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>64</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>12</v>
@@ -1978,71 +1924,187 @@
       <c r="G30" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H30" s="37" t="s">
+      <c r="H30" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="37" t="s">
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="O30" s="38"/>
-      <c r="P30" s="38"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="38"/>
-      <c r="U30" s="38"/>
-      <c r="V30" s="38"/>
-      <c r="W30" s="38"/>
-      <c r="X30" s="38"/>
-      <c r="Y30" s="38"/>
-      <c r="Z30" s="38"/>
-      <c r="AA30" s="38"/>
-      <c r="AB30" s="38"/>
-      <c r="AC30" s="38"/>
-      <c r="AD30" s="38"/>
-      <c r="AE30" s="38"/>
-      <c r="AF30" s="38"/>
-      <c r="AG30" s="38"/>
-      <c r="AH30" s="38"/>
-      <c r="AI30" s="38"/>
-      <c r="AJ30" s="38"/>
-      <c r="AK30" s="38"/>
-      <c r="AL30" s="38"/>
-      <c r="AM30" s="38"/>
-      <c r="AN30" s="38"/>
-      <c r="AO30" s="39"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="36"/>
+      <c r="V30" s="36"/>
+      <c r="W30" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
+      <c r="AA30" s="36"/>
+      <c r="AB30" s="36"/>
+      <c r="AC30" s="36"/>
+      <c r="AD30" s="36"/>
+      <c r="AE30" s="36"/>
+      <c r="AF30" s="36"/>
+      <c r="AG30" s="36"/>
+      <c r="AH30" s="36"/>
+      <c r="AI30" s="36"/>
+      <c r="AJ30" s="36"/>
+      <c r="AK30" s="36"/>
+      <c r="AL30" s="36"/>
+      <c r="AM30" s="36"/>
+      <c r="AN30" s="36"/>
+      <c r="AO30" s="37"/>
       <c r="AQ30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D31" s="21"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
+      <c r="V31" s="36"/>
+      <c r="W31" s="36"/>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="36"/>
+      <c r="AC31" s="36"/>
+      <c r="AD31" s="36"/>
+      <c r="AE31" s="36"/>
+      <c r="AF31" s="36"/>
+      <c r="AG31" s="36"/>
+      <c r="AH31" s="36"/>
+      <c r="AI31" s="36"/>
+      <c r="AJ31" s="36"/>
+      <c r="AK31" s="36"/>
+      <c r="AL31" s="36"/>
+      <c r="AM31" s="36"/>
+      <c r="AN31" s="36"/>
+      <c r="AO31" s="37"/>
+      <c r="AQ31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="36"/>
+      <c r="U32" s="36"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="36"/>
+      <c r="Y32" s="36"/>
+      <c r="Z32" s="36"/>
+      <c r="AA32" s="36"/>
+      <c r="AB32" s="36"/>
+      <c r="AC32" s="36"/>
+      <c r="AD32" s="36"/>
+      <c r="AE32" s="36"/>
+      <c r="AF32" s="36"/>
+      <c r="AG32" s="36"/>
+      <c r="AH32" s="36"/>
+      <c r="AI32" s="36"/>
+      <c r="AJ32" s="36"/>
+      <c r="AK32" s="36"/>
+      <c r="AL32" s="36"/>
+      <c r="AM32" s="36"/>
+      <c r="AN32" s="36"/>
+      <c r="AO32" s="37"/>
+      <c r="AQ32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D33" s="21"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="N29:AO29"/>
-    <mergeCell ref="N30:AO30"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="N28:AO28"/>
     <mergeCell ref="F4:AH4"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="G7:AH7"/>
-    <mergeCell ref="H27:AH27"/>
-    <mergeCell ref="F26:AH26"/>
+    <mergeCell ref="H29:AH29"/>
+    <mergeCell ref="F28:AH28"/>
+    <mergeCell ref="N31:AO31"/>
+    <mergeCell ref="N32:AO32"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="N30:AO30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add dfu packets to serial packet diagram
</commit_message>
<xml_diff>
--- a/docs/serial_interface.xlsx
+++ b/docs/serial_interface.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trsn\Documents\SDK8\examples\nrf51-ble-bcast-mesh\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="180" windowWidth="17520" windowHeight="12645"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
   <si>
     <t>Commands</t>
   </si>
@@ -153,9 +158,6 @@
     <t>CMD_RSP w/adv_int</t>
   </si>
   <si>
-    <t>H: Value handle, T: address type (e.g. BLE, IP)</t>
-  </si>
-  <si>
     <t>H: Value handle</t>
   </si>
   <si>
@@ -289,12 +291,27 @@
   </si>
   <si>
     <t>EVENT_TX</t>
+  </si>
+  <si>
+    <t>DFU data</t>
+  </si>
+  <si>
+    <t>dfu_data</t>
+  </si>
+  <si>
+    <t>CMD_RSP w/DFU</t>
+  </si>
+  <si>
+    <t>0x78</t>
+  </si>
+  <si>
+    <t>1..26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -485,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -549,9 +566,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,31 +590,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -608,12 +598,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -626,6 +610,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -637,6 +624,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -647,6 +667,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -695,7 +718,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -730,7 +753,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -939,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AQ44"/>
+  <dimension ref="A2:AQ46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:AD7"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,15 +973,15 @@
     <col min="1" max="1" width="3.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="49" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="38" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="42" width="2.85546875" style="2" customWidth="1"/>
     <col min="43" max="43" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:43" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="44" t="s">
-        <v>49</v>
+      <c r="B2" s="35" t="s">
+        <v>48</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -1082,7 +1105,7 @@
       <c r="C3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="39" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1116,37 +1139,37 @@
       <c r="E4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="39"/>
-      <c r="AD4" s="39"/>
-      <c r="AE4" s="39"/>
-      <c r="AF4" s="39"/>
-      <c r="AG4" s="39"/>
-      <c r="AH4" s="40"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
+      <c r="V4" s="51"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="51"/>
+      <c r="Y4" s="51"/>
+      <c r="Z4" s="51"/>
+      <c r="AA4" s="51"/>
+      <c r="AB4" s="51"/>
+      <c r="AC4" s="51"/>
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="51"/>
+      <c r="AF4" s="51"/>
+      <c r="AG4" s="51"/>
+      <c r="AH4" s="52"/>
       <c r="AI4" s="16"/>
       <c r="AJ4" s="17"/>
       <c r="AK4" s="17"/>
@@ -1158,16 +1181,16 @@
     </row>
     <row r="5" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="D5" s="22">
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
@@ -1178,7 +1201,7 @@
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
-      <c r="O5" s="29"/>
+      <c r="O5" s="28"/>
       <c r="P5" s="17"/>
       <c r="Q5" s="17"/>
       <c r="R5" s="17"/>
@@ -1207,7 +1230,7 @@
       <c r="AO5" s="17"/>
       <c r="AP5" s="17"/>
       <c r="AQ5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:43" x14ac:dyDescent="0.25">
@@ -1223,30 +1246,30 @@
       <c r="E6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="37"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="48"/>
       <c r="N6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="31"/>
-      <c r="P6" s="24"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="25"/>
-      <c r="AG6" s="25"/>
-      <c r="AH6" s="25"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="23"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="24"/>
       <c r="AI6" s="7"/>
       <c r="AQ6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:43" x14ac:dyDescent="0.25">
@@ -1257,46 +1280,46 @@
         <v>12</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34" t="s">
+      <c r="G7" s="41"/>
+      <c r="H7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="34"/>
-      <c r="AC7" s="34"/>
-      <c r="AD7" s="34"/>
-      <c r="AE7" s="33"/>
-      <c r="AF7" s="30"/>
-      <c r="AG7" s="30"/>
-      <c r="AH7" s="30"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
+      <c r="AE7" s="32"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29"/>
       <c r="AQ7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:43" x14ac:dyDescent="0.25">
@@ -1312,12 +1335,12 @@
       <c r="E8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="34"/>
+      <c r="G8" s="41"/>
       <c r="AQ8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:43" x14ac:dyDescent="0.25">
@@ -1333,17 +1356,17 @@
       <c r="E9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="34"/>
+      <c r="G9" s="41"/>
       <c r="AQ9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1352,13 +1375,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="26"/>
+        <v>61</v>
+      </c>
+      <c r="F10" s="25"/>
     </row>
     <row r="11" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1367,13 +1390,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="26"/>
+        <v>62</v>
+      </c>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1382,116 +1405,116 @@
         <v>5</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="27" t="s">
+      <c r="G12" s="41"/>
+      <c r="H12" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
       <c r="AQ12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="10">
         <v>4</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="28" t="s">
-        <v>71</v>
+      <c r="G13" s="57"/>
+      <c r="H13" s="31" t="s">
+        <v>70</v>
       </c>
       <c r="AQ13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="D14" s="15"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
+      <c r="AC14" s="41"/>
+      <c r="AD14" s="41"/>
     </row>
     <row r="15" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="11">
-        <v>3</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="7"/>
-      <c r="AE15" s="7"/>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
-      <c r="AH15" s="7"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="D16" s="11">
+        <v>3</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="41"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -1522,19 +1545,17 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+        <v>34</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -1565,16 +1586,16 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="10">
         <v>1</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -1608,16 +1629,16 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" s="10">
         <v>1</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1650,8 +1671,18 @@
       <c r="AH19" s="7"/>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D20" s="48"/>
-      <c r="E20" s="12"/>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -1683,7 +1714,7 @@
       <c r="AH20" s="7"/>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D21" s="48"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="12"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1716,7 +1747,7 @@
       <c r="AH21" s="7"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D22" s="48"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="12"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -1749,7 +1780,7 @@
       <c r="AH22" s="7"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D23" s="48"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="12"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -1782,269 +1813,267 @@
       <c r="AH23" s="7"/>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D24" s="48"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="12"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+      <c r="AE24" s="7"/>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="7"/>
+      <c r="AH24" s="7"/>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="D25" s="48"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="12"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="AI25" s="7"/>
-      <c r="AJ25" s="7"/>
-      <c r="AK25" s="7"/>
-      <c r="AL25" s="7"/>
-      <c r="AM25" s="7"/>
-      <c r="AN25" s="7"/>
-      <c r="AO25" s="7"/>
-      <c r="AP25" s="7"/>
-    </row>
-    <row r="26" spans="1:43" ht="23.25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="AI26" s="19"/>
-      <c r="AJ26" s="19"/>
-      <c r="AK26" s="19"/>
-      <c r="AL26" s="19"/>
-      <c r="AM26" s="19"/>
-      <c r="AN26" s="19"/>
-      <c r="AO26" s="19"/>
-      <c r="AP26" s="19"/>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="D26" s="37"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="AI26" s="7"/>
+      <c r="AJ26" s="7"/>
+      <c r="AK26" s="7"/>
+      <c r="AL26" s="7"/>
+      <c r="AM26" s="7"/>
+      <c r="AN26" s="7"/>
+      <c r="AO26" s="7"/>
+      <c r="AP26" s="7"/>
+    </row>
+    <row r="27" spans="1:43" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="AI27" s="19"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
+      <c r="AL27" s="19"/>
+      <c r="AM27" s="19"/>
+      <c r="AN27" s="19"/>
+      <c r="AO27" s="19"/>
+      <c r="AP27" s="19"/>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="17"/>
-      <c r="V27" s="17"/>
-      <c r="W27" s="17"/>
-      <c r="X27" s="17"/>
-      <c r="Y27" s="17"/>
-      <c r="Z27" s="17"/>
-      <c r="AA27" s="17"/>
-      <c r="AB27" s="17"/>
-      <c r="AC27" s="17"/>
-      <c r="AD27" s="17"/>
-      <c r="AE27" s="17"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="17"/>
-      <c r="AH27" s="17"/>
-      <c r="AI27" s="17"/>
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
-      <c r="AL27" s="17"/>
-      <c r="AM27" s="17"/>
-      <c r="AN27" s="17"/>
-      <c r="AO27" s="17"/>
-      <c r="AP27" s="17"/>
-    </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="10">
-        <v>4</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28" s="6"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
-      <c r="Z28" s="24"/>
-      <c r="AA28" s="24"/>
-      <c r="AB28" s="24"/>
-      <c r="AC28" s="24"/>
-      <c r="AD28" s="24"/>
-      <c r="AE28" s="30"/>
-      <c r="AF28" s="30"/>
-      <c r="AG28" s="30"/>
-      <c r="AH28" s="30"/>
-      <c r="AI28" s="25"/>
-      <c r="AQ28" t="s">
-        <v>59</v>
-      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="17"/>
+      <c r="AF28" s="17"/>
+      <c r="AG28" s="17"/>
+      <c r="AH28" s="17"/>
+      <c r="AI28" s="17"/>
+      <c r="AJ28" s="17"/>
+      <c r="AK28" s="17"/>
+      <c r="AL28" s="17"/>
+      <c r="AM28" s="17"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="10">
+        <v>4</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+      <c r="AA29" s="23"/>
+      <c r="AB29" s="23"/>
+      <c r="AC29" s="23"/>
+      <c r="AD29" s="23"/>
+      <c r="AE29" s="29"/>
+      <c r="AF29" s="29"/>
+      <c r="AG29" s="29"/>
+      <c r="AH29" s="29"/>
+      <c r="AI29" s="24"/>
+      <c r="AQ29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="10" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="38" t="s">
+      <c r="F30" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-      <c r="X29" s="39"/>
-      <c r="Y29" s="39"/>
-      <c r="Z29" s="39"/>
-      <c r="AA29" s="39"/>
-      <c r="AB29" s="39"/>
-      <c r="AC29" s="39"/>
-      <c r="AD29" s="39"/>
-      <c r="AE29" s="39"/>
-      <c r="AF29" s="39"/>
-      <c r="AG29" s="39"/>
-      <c r="AH29" s="40"/>
-      <c r="AI29" s="30"/>
-      <c r="AK29"/>
-      <c r="AL29"/>
-      <c r="AM29"/>
-      <c r="AN29"/>
-      <c r="AO29"/>
-      <c r="AP29"/>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="36"/>
-      <c r="O30" s="36"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36"/>
-      <c r="R30" s="36"/>
-      <c r="S30" s="36"/>
-      <c r="T30" s="36"/>
-      <c r="U30" s="36"/>
-      <c r="V30" s="36"/>
-      <c r="W30" s="36"/>
-      <c r="X30" s="36"/>
-      <c r="Y30" s="36"/>
-      <c r="Z30" s="36"/>
-      <c r="AA30" s="36"/>
-      <c r="AB30" s="36"/>
-      <c r="AC30" s="36"/>
-      <c r="AD30" s="36"/>
-      <c r="AE30" s="36"/>
-      <c r="AF30" s="37"/>
-      <c r="AG30" s="30"/>
-      <c r="AH30" s="30"/>
-      <c r="AI30" s="30"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="51"/>
+      <c r="V30" s="51"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="51"/>
+      <c r="Z30" s="51"/>
+      <c r="AA30" s="51"/>
+      <c r="AB30" s="51"/>
+      <c r="AC30" s="51"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="51"/>
+      <c r="AF30" s="51"/>
+      <c r="AG30" s="51"/>
+      <c r="AH30" s="52"/>
+      <c r="AI30" s="29"/>
       <c r="AK30"/>
       <c r="AL30"/>
       <c r="AM30"/>
       <c r="AN30"/>
       <c r="AO30"/>
       <c r="AP30"/>
-      <c r="AQ30" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="10">
-        <v>7</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" s="47"/>
-      <c r="J31" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="K31" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE31" s="30"/>
-      <c r="AF31" s="30"/>
-      <c r="AG31" s="30"/>
-      <c r="AH31" s="30"/>
-      <c r="AI31" s="30"/>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+      <c r="U31" s="49"/>
+      <c r="V31" s="49"/>
+      <c r="W31" s="49"/>
+      <c r="X31" s="49"/>
+      <c r="Y31" s="49"/>
+      <c r="Z31" s="49"/>
+      <c r="AA31" s="49"/>
+      <c r="AB31" s="49"/>
+      <c r="AC31" s="49"/>
+      <c r="AD31" s="49"/>
+      <c r="AE31" s="49"/>
+      <c r="AF31" s="48"/>
+      <c r="AG31" s="29"/>
+      <c r="AH31" s="29"/>
+      <c r="AI31" s="29"/>
       <c r="AK31"/>
       <c r="AL31"/>
       <c r="AM31"/>
@@ -2052,311 +2081,370 @@
       <c r="AO31"/>
       <c r="AP31"/>
       <c r="AQ31" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="H32" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="10">
+        <v>7</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="34"/>
-      <c r="J32" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="36"/>
-      <c r="U32" s="36"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="36"/>
-      <c r="AA32" s="36"/>
-      <c r="AB32" s="36"/>
-      <c r="AC32" s="36"/>
-      <c r="AD32" s="36"/>
-      <c r="AE32" s="36"/>
-      <c r="AF32" s="37"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="K32" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE32" s="29"/>
+      <c r="AF32" s="29"/>
+      <c r="AG32" s="29"/>
+      <c r="AH32" s="29"/>
+      <c r="AI32" s="29"/>
+      <c r="AK32"/>
+      <c r="AL32"/>
+      <c r="AM32"/>
+      <c r="AN32"/>
+      <c r="AO32"/>
+      <c r="AP32"/>
+      <c r="AQ32" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="33" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="10">
-        <v>6</v>
-      </c>
-      <c r="H33" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="J33" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>80</v>
       </c>
+      <c r="H33" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="41"/>
+      <c r="J33" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="49"/>
+      <c r="V33" s="49"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="49"/>
+      <c r="Y33" s="49"/>
+      <c r="Z33" s="49"/>
+      <c r="AA33" s="49"/>
+      <c r="AB33" s="49"/>
+      <c r="AC33" s="49"/>
+      <c r="AD33" s="49"/>
+      <c r="AE33" s="49"/>
+      <c r="AF33" s="48"/>
     </row>
     <row r="34" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="D34" s="10">
-        <v>7</v>
-      </c>
-      <c r="H34" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
+        <v>6</v>
+      </c>
+      <c r="H34" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="J34" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ34" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="35" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="D35" s="10">
-        <v>4</v>
-      </c>
-      <c r="H35" s="32" t="s">
-        <v>16</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H35" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
     </row>
     <row r="36" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="D36" s="10">
+        <v>4</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="10">
         <v>7</v>
       </c>
-      <c r="H36" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-    </row>
-    <row r="37" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="34" t="s">
+      <c r="H37" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="41"/>
+    </row>
+    <row r="38" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="10">
+        <v>5</v>
+      </c>
+      <c r="H38" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G37" s="34"/>
-      <c r="H37" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="36"/>
-      <c r="O37" s="36"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="T37" s="36"/>
-      <c r="U37" s="36"/>
-      <c r="V37" s="36"/>
-      <c r="W37" s="36"/>
-      <c r="X37" s="36"/>
-      <c r="Y37" s="36"/>
-      <c r="Z37" s="36"/>
-      <c r="AA37" s="36"/>
-      <c r="AB37" s="36"/>
-      <c r="AC37" s="36"/>
-      <c r="AD37" s="37"/>
-      <c r="AQ37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="34"/>
-      <c r="H38" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="36"/>
-      <c r="O38" s="36"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="36"/>
-      <c r="R38" s="36"/>
-      <c r="S38" s="36"/>
-      <c r="T38" s="36"/>
-      <c r="U38" s="36"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="36"/>
-      <c r="X38" s="36"/>
-      <c r="Y38" s="36"/>
-      <c r="Z38" s="36"/>
-      <c r="AA38" s="36"/>
-      <c r="AB38" s="36"/>
-      <c r="AC38" s="36"/>
-      <c r="AD38" s="37"/>
+      <c r="I38" s="41"/>
       <c r="AQ38" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="37"/>
-      <c r="H39" s="35" t="s">
+      <c r="G39" s="41"/>
+      <c r="H39" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="36"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="36"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="36"/>
-      <c r="AA39" s="36"/>
-      <c r="AB39" s="36"/>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="37"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="49"/>
+      <c r="U39" s="49"/>
+      <c r="V39" s="49"/>
+      <c r="W39" s="49"/>
+      <c r="X39" s="49"/>
+      <c r="Y39" s="49"/>
+      <c r="Z39" s="49"/>
+      <c r="AA39" s="49"/>
+      <c r="AB39" s="49"/>
+      <c r="AC39" s="49"/>
+      <c r="AD39" s="48"/>
       <c r="AQ39" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="37"/>
-      <c r="H40" s="35" t="s">
+      <c r="G40" s="41"/>
+      <c r="H40" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="36"/>
-      <c r="T40" s="36"/>
-      <c r="U40" s="36"/>
-      <c r="V40" s="36"/>
-      <c r="W40" s="36"/>
-      <c r="X40" s="36"/>
-      <c r="Y40" s="36"/>
-      <c r="Z40" s="36"/>
-      <c r="AA40" s="36"/>
-      <c r="AB40" s="36"/>
-      <c r="AC40" s="36"/>
-      <c r="AD40" s="37"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="49"/>
+      <c r="U40" s="49"/>
+      <c r="V40" s="49"/>
+      <c r="W40" s="49"/>
+      <c r="X40" s="49"/>
+      <c r="Y40" s="49"/>
+      <c r="Z40" s="49"/>
+      <c r="AA40" s="49"/>
+      <c r="AB40" s="49"/>
+      <c r="AC40" s="49"/>
+      <c r="AD40" s="48"/>
       <c r="AQ40" t="s">
         <v>45</v>
       </c>
     </row>
+    <row r="41" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="48"/>
+      <c r="H41" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="49"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="49"/>
+      <c r="U41" s="49"/>
+      <c r="V41" s="49"/>
+      <c r="W41" s="49"/>
+      <c r="X41" s="49"/>
+      <c r="Y41" s="49"/>
+      <c r="Z41" s="49"/>
+      <c r="AA41" s="49"/>
+      <c r="AB41" s="49"/>
+      <c r="AC41" s="49"/>
+      <c r="AD41" s="48"/>
+      <c r="AQ41" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="42" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B42" s="52" t="s">
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="48"/>
+      <c r="H42" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="49"/>
+      <c r="U42" s="49"/>
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49"/>
+      <c r="Y42" s="49"/>
+      <c r="Z42" s="49"/>
+      <c r="AA42" s="49"/>
+      <c r="AB42" s="49"/>
+      <c r="AC42" s="49"/>
+      <c r="AD42" s="48"/>
+      <c r="AQ42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B44" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="43"/>
+      <c r="D44" s="44"/>
+    </row>
+    <row r="45" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B45" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="46"/>
+      <c r="D45" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B46" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="53"/>
-      <c r="D42" s="54"/>
-    </row>
-    <row r="43" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B43" s="55" t="s">
+      <c r="C46" s="46"/>
+      <c r="D46" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="D43" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B44" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="56"/>
-      <c r="D44" s="10" t="s">
-        <v>87</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
+  <mergeCells count="30">
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H41:AD41"/>
+    <mergeCell ref="H40:AD40"/>
+    <mergeCell ref="F30:AH30"/>
+    <mergeCell ref="H39:AD39"/>
+    <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:AD40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:AF33"/>
+    <mergeCell ref="H31:AF31"/>
+    <mergeCell ref="F14:AD14"/>
+    <mergeCell ref="H38:I38"/>
     <mergeCell ref="F4:AH4"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:G7"/>
@@ -2364,20 +2452,13 @@
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H7:AD7"/>
     <mergeCell ref="J6:M6"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H39:AD39"/>
-    <mergeCell ref="H38:AD38"/>
-    <mergeCell ref="F29:AH29"/>
-    <mergeCell ref="H37:AD37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:AF32"/>
-    <mergeCell ref="H30:AF30"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:AD42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Improve Serial interface docs
</commit_message>
<xml_diff>
--- a/docs/serial_interface.xlsx
+++ b/docs/serial_interface.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
   <si>
     <t>Commands</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>1..26</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -515,9 +518,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -613,6 +613,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,39 +660,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -964,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AQ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,14 +976,14 @@
     <col min="1" max="1" width="3.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="37" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="42" width="2.85546875" style="2" customWidth="1"/>
     <col min="43" max="43" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:43" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="2">
@@ -1105,23 +1108,23 @@
       <c r="C3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="38" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7"/>
-      <c r="AL3" s="7"/>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7"/>
-      <c r="AP3" s="7"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6"/>
+      <c r="AM3" s="6"/>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
       <c r="AQ3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1133,51 +1136,51 @@
       <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="51"/>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="51"/>
-      <c r="Z4" s="51"/>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="51"/>
-      <c r="AC4" s="51"/>
-      <c r="AD4" s="51"/>
-      <c r="AE4" s="51"/>
-      <c r="AF4" s="51"/>
-      <c r="AG4" s="51"/>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="17"/>
-      <c r="AK4" s="17"/>
-      <c r="AL4" s="17"/>
-      <c r="AM4" s="17"/>
-      <c r="AN4" s="17"/>
-      <c r="AO4" s="17"/>
-      <c r="AP4" s="17"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="47"/>
+      <c r="AE4" s="47"/>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="16"/>
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16"/>
     </row>
     <row r="5" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
@@ -1186,49 +1189,49 @@
       <c r="C5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>1</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="17"/>
-      <c r="AB5" s="17"/>
-      <c r="AC5" s="17"/>
-      <c r="AD5" s="17"/>
-      <c r="AE5" s="17"/>
-      <c r="AF5" s="17"/>
-      <c r="AG5" s="17"/>
-      <c r="AH5" s="17"/>
-      <c r="AI5" s="17"/>
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
-      <c r="AL5" s="17"/>
-      <c r="AM5" s="17"/>
-      <c r="AN5" s="17"/>
-      <c r="AO5" s="17"/>
-      <c r="AP5" s="17"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="16"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="16"/>
+      <c r="AP5" s="16"/>
       <c r="AQ5" s="5" t="s">
         <v>53</v>
       </c>
@@ -1240,34 +1243,34 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>10</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="47" t="s">
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="48"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="45"/>
       <c r="N6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="30"/>
-      <c r="P6" s="23"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
-      <c r="AI6" s="7"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="22"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+      <c r="AI6" s="6"/>
       <c r="AQ6" t="s">
         <v>64</v>
       </c>
@@ -1279,45 +1282,45 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41" t="s">
+      <c r="G7" s="42"/>
+      <c r="H7" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="41"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="41"/>
-      <c r="AC7" s="41"/>
-      <c r="AD7" s="41"/>
-      <c r="AE7" s="32"/>
-      <c r="AF7" s="29"/>
-      <c r="AG7" s="29"/>
-      <c r="AH7" s="29"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="42"/>
+      <c r="Z7" s="42"/>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="42"/>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="42"/>
+      <c r="AE7" s="31"/>
+      <c r="AF7" s="28"/>
+      <c r="AG7" s="28"/>
+      <c r="AH7" s="28"/>
       <c r="AQ7" t="s">
         <v>45</v>
       </c>
@@ -1329,16 +1332,16 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>3</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="41"/>
+      <c r="G8" s="42"/>
       <c r="AQ8" t="s">
         <v>45</v>
       </c>
@@ -1350,16 +1353,16 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>3</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="41"/>
+      <c r="G9" s="42"/>
       <c r="AQ9" t="s">
         <v>45</v>
       </c>
@@ -1371,13 +1374,13 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>1</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1386,13 +1389,13 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1401,28 +1404,28 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>5</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="41" t="s">
+      <c r="F12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="26" t="s">
+      <c r="G12" s="42"/>
+      <c r="H12" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
       <c r="AQ12" t="s">
         <v>76</v>
       </c>
@@ -1434,17 +1437,17 @@
       <c r="C13" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>4</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="31" t="s">
+      <c r="G13" s="41"/>
+      <c r="H13" s="30" t="s">
         <v>70</v>
       </c>
       <c r="AQ13" t="s">
@@ -1458,45 +1461,45 @@
       <c r="C14" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="41"/>
-      <c r="AD14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="42"/>
+      <c r="X14" s="42"/>
+      <c r="Y14" s="42"/>
+      <c r="Z14" s="42"/>
+      <c r="AA14" s="42"/>
+      <c r="AB14" s="42"/>
+      <c r="AC14" s="42"/>
+      <c r="AD14" s="42"/>
     </row>
     <row r="15" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="D15" s="15"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1505,43 +1508,43 @@
       <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>3</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="41"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="7"/>
-      <c r="AE16" s="7"/>
-      <c r="AF16" s="7"/>
-      <c r="AG16" s="7"/>
-      <c r="AH16" s="7"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="6"/>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -1550,39 +1553,39 @@
       <c r="C17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>1</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="7"/>
-      <c r="AF17" s="7"/>
-      <c r="AG17" s="7"/>
-      <c r="AH17" s="7"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -1591,41 +1594,41 @@
       <c r="C18" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>1</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="7"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="7"/>
-      <c r="AD18" s="7"/>
-      <c r="AE18" s="7"/>
-      <c r="AF18" s="7"/>
-      <c r="AG18" s="7"/>
-      <c r="AH18" s="7"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="6"/>
+      <c r="AG18" s="6"/>
+      <c r="AH18" s="6"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1634,41 +1637,41 @@
       <c r="C19" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>1</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
-      <c r="AC19" s="7"/>
-      <c r="AD19" s="7"/>
-      <c r="AE19" s="7"/>
-      <c r="AF19" s="7"/>
-      <c r="AG19" s="7"/>
-      <c r="AH19" s="7"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="6"/>
+      <c r="AH19" s="6"/>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -1677,212 +1680,212 @@
       <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>1</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="7"/>
-      <c r="AB20" s="7"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
-      <c r="AE20" s="7"/>
-      <c r="AF20" s="7"/>
-      <c r="AG20" s="7"/>
-      <c r="AH20" s="7"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D21" s="37"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
-      <c r="AB21" s="7"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D22" s="37"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
-      <c r="AA22" s="7"/>
-      <c r="AB22" s="7"/>
-      <c r="AC22" s="7"/>
-      <c r="AD22" s="7"/>
-      <c r="AE22" s="7"/>
-      <c r="AF22" s="7"/>
-      <c r="AG22" s="7"/>
-      <c r="AH22" s="7"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6"/>
+      <c r="AH22" s="6"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D23" s="37"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
-      <c r="AE23" s="7"/>
-      <c r="AF23" s="7"/>
-      <c r="AG23" s="7"/>
-      <c r="AH23" s="7"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6"/>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D24" s="37"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="7"/>
-      <c r="AB24" s="7"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
-      <c r="AE24" s="7"/>
-      <c r="AF24" s="7"/>
-      <c r="AG24" s="7"/>
-      <c r="AH24" s="7"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="6"/>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="D25" s="37"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="AI26" s="7"/>
-      <c r="AJ26" s="7"/>
-      <c r="AK26" s="7"/>
-      <c r="AL26" s="7"/>
-      <c r="AM26" s="7"/>
-      <c r="AN26" s="7"/>
-      <c r="AO26" s="7"/>
-      <c r="AP26" s="7"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="AI26" s="6"/>
+      <c r="AJ26" s="6"/>
+      <c r="AK26" s="6"/>
+      <c r="AL26" s="6"/>
+      <c r="AM26" s="6"/>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="6"/>
+      <c r="AP26" s="6"/>
     </row>
     <row r="27" spans="1:43" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="AI27" s="19"/>
-      <c r="AJ27" s="19"/>
-      <c r="AK27" s="19"/>
-      <c r="AL27" s="19"/>
-      <c r="AM27" s="19"/>
-      <c r="AN27" s="19"/>
-      <c r="AO27" s="19"/>
-      <c r="AP27" s="19"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="AI27" s="18"/>
+      <c r="AJ27" s="18"/>
+      <c r="AK27" s="18"/>
+      <c r="AL27" s="18"/>
+      <c r="AM27" s="18"/>
+      <c r="AN27" s="18"/>
+      <c r="AO27" s="18"/>
+      <c r="AP27" s="18"/>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
@@ -1890,51 +1893,51 @@
         <v>11</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="17"/>
-      <c r="V28" s="17"/>
-      <c r="W28" s="17"/>
-      <c r="X28" s="17"/>
-      <c r="Y28" s="17"/>
-      <c r="Z28" s="17"/>
-      <c r="AA28" s="17"/>
-      <c r="AB28" s="17"/>
-      <c r="AC28" s="17"/>
-      <c r="AD28" s="17"/>
-      <c r="AE28" s="17"/>
-      <c r="AF28" s="17"/>
-      <c r="AG28" s="17"/>
-      <c r="AH28" s="17"/>
-      <c r="AI28" s="17"/>
-      <c r="AJ28" s="17"/>
-      <c r="AK28" s="17"/>
-      <c r="AL28" s="17"/>
-      <c r="AM28" s="17"/>
-      <c r="AN28" s="17"/>
-      <c r="AO28" s="17"/>
-      <c r="AP28" s="17"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="16"/>
+      <c r="AB28" s="16"/>
+      <c r="AC28" s="16"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="16"/>
+      <c r="AF28" s="16"/>
+      <c r="AG28" s="16"/>
+      <c r="AH28" s="16"/>
+      <c r="AI28" s="16"/>
+      <c r="AJ28" s="16"/>
+      <c r="AK28" s="16"/>
+      <c r="AL28" s="16"/>
+      <c r="AM28" s="16"/>
+      <c r="AN28" s="16"/>
+      <c r="AO28" s="16"/>
+      <c r="AP28" s="16"/>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <v>4</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>57</v>
       </c>
       <c r="F29" s="3" t="s">
@@ -1943,34 +1946,36 @@
       <c r="G29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="23"/>
-      <c r="Z29" s="23"/>
-      <c r="AA29" s="23"/>
-      <c r="AB29" s="23"/>
-      <c r="AC29" s="23"/>
-      <c r="AD29" s="23"/>
-      <c r="AE29" s="29"/>
-      <c r="AF29" s="29"/>
-      <c r="AG29" s="29"/>
-      <c r="AH29" s="29"/>
-      <c r="AI29" s="24"/>
+      <c r="H29" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+      <c r="AD29" s="22"/>
+      <c r="AE29" s="28"/>
+      <c r="AF29" s="28"/>
+      <c r="AG29" s="28"/>
+      <c r="AH29" s="28"/>
+      <c r="AI29" s="23"/>
       <c r="AQ29" t="s">
         <v>58</v>
       </c>
@@ -1980,44 +1985,44 @@
         <v>19</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="50" t="s">
+      <c r="F30" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="51"/>
-      <c r="T30" s="51"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="51"/>
-      <c r="W30" s="51"/>
-      <c r="X30" s="51"/>
-      <c r="Y30" s="51"/>
-      <c r="Z30" s="51"/>
-      <c r="AA30" s="51"/>
-      <c r="AB30" s="51"/>
-      <c r="AC30" s="51"/>
-      <c r="AD30" s="51"/>
-      <c r="AE30" s="51"/>
-      <c r="AF30" s="51"/>
-      <c r="AG30" s="51"/>
-      <c r="AH30" s="52"/>
-      <c r="AI30" s="29"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+      <c r="P30" s="47"/>
+      <c r="Q30" s="47"/>
+      <c r="R30" s="47"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="47"/>
+      <c r="V30" s="47"/>
+      <c r="W30" s="47"/>
+      <c r="X30" s="47"/>
+      <c r="Y30" s="47"/>
+      <c r="Z30" s="47"/>
+      <c r="AA30" s="47"/>
+      <c r="AB30" s="47"/>
+      <c r="AC30" s="47"/>
+      <c r="AD30" s="47"/>
+      <c r="AE30" s="47"/>
+      <c r="AF30" s="47"/>
+      <c r="AG30" s="47"/>
+      <c r="AH30" s="48"/>
+      <c r="AI30" s="28"/>
       <c r="AK30"/>
       <c r="AL30"/>
       <c r="AM30"/>
@@ -2029,51 +2034,51 @@
       <c r="B31" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="31" t="s">
+      <c r="F31" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="47" t="s">
+      <c r="H31" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-      <c r="T31" s="49"/>
-      <c r="U31" s="49"/>
-      <c r="V31" s="49"/>
-      <c r="W31" s="49"/>
-      <c r="X31" s="49"/>
-      <c r="Y31" s="49"/>
-      <c r="Z31" s="49"/>
-      <c r="AA31" s="49"/>
-      <c r="AB31" s="49"/>
-      <c r="AC31" s="49"/>
-      <c r="AD31" s="49"/>
-      <c r="AE31" s="49"/>
-      <c r="AF31" s="48"/>
-      <c r="AG31" s="29"/>
-      <c r="AH31" s="29"/>
-      <c r="AI31" s="29"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
+      <c r="P31" s="44"/>
+      <c r="Q31" s="44"/>
+      <c r="R31" s="44"/>
+      <c r="S31" s="44"/>
+      <c r="T31" s="44"/>
+      <c r="U31" s="44"/>
+      <c r="V31" s="44"/>
+      <c r="W31" s="44"/>
+      <c r="X31" s="44"/>
+      <c r="Y31" s="44"/>
+      <c r="Z31" s="44"/>
+      <c r="AA31" s="44"/>
+      <c r="AB31" s="44"/>
+      <c r="AC31" s="44"/>
+      <c r="AD31" s="44"/>
+      <c r="AE31" s="44"/>
+      <c r="AF31" s="45"/>
+      <c r="AG31" s="28"/>
+      <c r="AH31" s="28"/>
+      <c r="AI31" s="28"/>
       <c r="AK31"/>
       <c r="AL31"/>
       <c r="AM31"/>
@@ -2088,27 +2093,27 @@
       <c r="C32" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="9">
         <v>7</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="55" t="s">
+      <c r="E32" s="12"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="56"/>
-      <c r="J32" s="34" t="s">
+      <c r="I32" s="50"/>
+      <c r="J32" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="K32" s="34" t="s">
+      <c r="K32" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="AE32" s="29"/>
-      <c r="AF32" s="29"/>
-      <c r="AG32" s="29"/>
-      <c r="AH32" s="29"/>
-      <c r="AI32" s="29"/>
+      <c r="AE32" s="28"/>
+      <c r="AF32" s="28"/>
+      <c r="AG32" s="28"/>
+      <c r="AH32" s="28"/>
+      <c r="AI32" s="28"/>
       <c r="AK32"/>
       <c r="AL32"/>
       <c r="AM32"/>
@@ -2123,53 +2128,53 @@
       <c r="C33" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="I33" s="41"/>
-      <c r="J33" s="47" t="s">
+      <c r="I33" s="42"/>
+      <c r="J33" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="49"/>
-      <c r="U33" s="49"/>
-      <c r="V33" s="49"/>
-      <c r="W33" s="49"/>
-      <c r="X33" s="49"/>
-      <c r="Y33" s="49"/>
-      <c r="Z33" s="49"/>
-      <c r="AA33" s="49"/>
-      <c r="AB33" s="49"/>
-      <c r="AC33" s="49"/>
-      <c r="AD33" s="49"/>
-      <c r="AE33" s="49"/>
-      <c r="AF33" s="48"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="44"/>
+      <c r="R33" s="44"/>
+      <c r="S33" s="44"/>
+      <c r="T33" s="44"/>
+      <c r="U33" s="44"/>
+      <c r="V33" s="44"/>
+      <c r="W33" s="44"/>
+      <c r="X33" s="44"/>
+      <c r="Y33" s="44"/>
+      <c r="Z33" s="44"/>
+      <c r="AA33" s="44"/>
+      <c r="AB33" s="44"/>
+      <c r="AC33" s="44"/>
+      <c r="AD33" s="44"/>
+      <c r="AE33" s="44"/>
+      <c r="AF33" s="45"/>
     </row>
     <row r="34" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="9">
         <v>6</v>
       </c>
-      <c r="H34" s="31" t="s">
+      <c r="H34" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="I34" s="31" t="s">
+      <c r="I34" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="J34" s="31" t="s">
+      <c r="J34" s="30" t="s">
         <v>78</v>
       </c>
       <c r="AQ34" t="s">
@@ -2180,24 +2185,24 @@
       <c r="C35" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="9">
         <v>7</v>
       </c>
-      <c r="H35" s="41" t="s">
+      <c r="H35" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="41"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
     </row>
     <row r="36" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="9">
         <v>4</v>
       </c>
-      <c r="H36" s="31" t="s">
+      <c r="H36" s="30" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2205,27 +2210,27 @@
       <c r="C37" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="9">
         <v>7</v>
       </c>
-      <c r="H37" s="41" t="s">
+      <c r="H37" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
     </row>
     <row r="38" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>91</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="9">
         <v>5</v>
       </c>
-      <c r="H38" s="41" t="s">
+      <c r="H38" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="I38" s="41"/>
+      <c r="I38" s="42"/>
       <c r="AQ38" t="s">
         <v>45</v>
       </c>
@@ -2234,41 +2239,41 @@
       <c r="B39" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="41" t="s">
+      <c r="F39" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="41"/>
-      <c r="H39" s="47" t="s">
+      <c r="G39" s="42"/>
+      <c r="H39" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
-      <c r="S39" s="49"/>
-      <c r="T39" s="49"/>
-      <c r="U39" s="49"/>
-      <c r="V39" s="49"/>
-      <c r="W39" s="49"/>
-      <c r="X39" s="49"/>
-      <c r="Y39" s="49"/>
-      <c r="Z39" s="49"/>
-      <c r="AA39" s="49"/>
-      <c r="AB39" s="49"/>
-      <c r="AC39" s="49"/>
-      <c r="AD39" s="48"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="44"/>
+      <c r="X39" s="44"/>
+      <c r="Y39" s="44"/>
+      <c r="Z39" s="44"/>
+      <c r="AA39" s="44"/>
+      <c r="AB39" s="44"/>
+      <c r="AC39" s="44"/>
+      <c r="AD39" s="45"/>
       <c r="AQ39" t="s">
         <v>45</v>
       </c>
@@ -2277,41 +2282,41 @@
       <c r="B40" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="41" t="s">
+      <c r="F40" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="41"/>
-      <c r="H40" s="47" t="s">
+      <c r="G40" s="42"/>
+      <c r="H40" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="49"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="49"/>
-      <c r="O40" s="49"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="49"/>
-      <c r="R40" s="49"/>
-      <c r="S40" s="49"/>
-      <c r="T40" s="49"/>
-      <c r="U40" s="49"/>
-      <c r="V40" s="49"/>
-      <c r="W40" s="49"/>
-      <c r="X40" s="49"/>
-      <c r="Y40" s="49"/>
-      <c r="Z40" s="49"/>
-      <c r="AA40" s="49"/>
-      <c r="AB40" s="49"/>
-      <c r="AC40" s="49"/>
-      <c r="AD40" s="48"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="44"/>
+      <c r="N40" s="44"/>
+      <c r="O40" s="44"/>
+      <c r="P40" s="44"/>
+      <c r="Q40" s="44"/>
+      <c r="R40" s="44"/>
+      <c r="S40" s="44"/>
+      <c r="T40" s="44"/>
+      <c r="U40" s="44"/>
+      <c r="V40" s="44"/>
+      <c r="W40" s="44"/>
+      <c r="X40" s="44"/>
+      <c r="Y40" s="44"/>
+      <c r="Z40" s="44"/>
+      <c r="AA40" s="44"/>
+      <c r="AB40" s="44"/>
+      <c r="AC40" s="44"/>
+      <c r="AD40" s="45"/>
       <c r="AQ40" t="s">
         <v>45</v>
       </c>
@@ -2320,41 +2325,41 @@
       <c r="B41" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="47" t="s">
+      <c r="F41" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="48"/>
-      <c r="H41" s="47" t="s">
+      <c r="G41" s="45"/>
+      <c r="H41" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I41" s="49"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="49"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="49"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
-      <c r="S41" s="49"/>
-      <c r="T41" s="49"/>
-      <c r="U41" s="49"/>
-      <c r="V41" s="49"/>
-      <c r="W41" s="49"/>
-      <c r="X41" s="49"/>
-      <c r="Y41" s="49"/>
-      <c r="Z41" s="49"/>
-      <c r="AA41" s="49"/>
-      <c r="AB41" s="49"/>
-      <c r="AC41" s="49"/>
-      <c r="AD41" s="48"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="44"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="44"/>
+      <c r="W41" s="44"/>
+      <c r="X41" s="44"/>
+      <c r="Y41" s="44"/>
+      <c r="Z41" s="44"/>
+      <c r="AA41" s="44"/>
+      <c r="AB41" s="44"/>
+      <c r="AC41" s="44"/>
+      <c r="AD41" s="45"/>
       <c r="AQ41" t="s">
         <v>45</v>
       </c>
@@ -2363,72 +2368,86 @@
       <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="47" t="s">
+      <c r="F42" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="48"/>
-      <c r="H42" s="47" t="s">
+      <c r="G42" s="45"/>
+      <c r="H42" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49"/>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="49"/>
-      <c r="S42" s="49"/>
-      <c r="T42" s="49"/>
-      <c r="U42" s="49"/>
-      <c r="V42" s="49"/>
-      <c r="W42" s="49"/>
-      <c r="X42" s="49"/>
-      <c r="Y42" s="49"/>
-      <c r="Z42" s="49"/>
-      <c r="AA42" s="49"/>
-      <c r="AB42" s="49"/>
-      <c r="AC42" s="49"/>
-      <c r="AD42" s="48"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="44"/>
+      <c r="S42" s="44"/>
+      <c r="T42" s="44"/>
+      <c r="U42" s="44"/>
+      <c r="V42" s="44"/>
+      <c r="W42" s="44"/>
+      <c r="X42" s="44"/>
+      <c r="Y42" s="44"/>
+      <c r="Z42" s="44"/>
+      <c r="AA42" s="44"/>
+      <c r="AB42" s="44"/>
+      <c r="AC42" s="44"/>
+      <c r="AD42" s="45"/>
       <c r="AQ42" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="44" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="44"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="55"/>
     </row>
     <row r="45" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B45" s="45" t="s">
+      <c r="B45" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="10" t="s">
+      <c r="C45" s="57"/>
+      <c r="D45" s="9" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="46" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="46"/>
-      <c r="D46" s="10" t="s">
+      <c r="C46" s="57"/>
+      <c r="D46" s="9" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:AD42"/>
+    <mergeCell ref="F4:AH4"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H7:AD7"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H41:AD41"/>
@@ -2445,20 +2464,6 @@
     <mergeCell ref="H31:AF31"/>
     <mergeCell ref="F14:AD14"/>
     <mergeCell ref="H38:I38"/>
-    <mergeCell ref="F4:AH4"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H7:AD7"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:AD42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>